<commit_message>
Added plot as an image.
</commit_message>
<xml_diff>
--- a/HICP_inflation_CZ.xlsx
+++ b/HICP_inflation_CZ.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>01/2022</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>10/2022</t>
+  </si>
+  <si>
+    <t>11/2022</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +472,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C12" si="0">B3/100</f>
+        <f t="shared" ref="C3:C13" si="0">B3/100</f>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D3" s="1">
@@ -505,7 +508,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D12" si="1">(C5+1)*D4</f>
+        <f t="shared" ref="D5:D13" si="1">(C5+1)*D4</f>
         <v>1.0797303619999998</v>
       </c>
     </row>
@@ -622,55 +625,68 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>1.3</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1676443971289576</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="3"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>

</xml_diff>